<commit_message>
add : RL-HL002 drawing
</commit_message>
<xml_diff>
--- a/機械設計/_BOM/RR-HL001.xlsx
+++ b/機械設計/_BOM/RR-HL001.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GitHub\2022-KawasakiRobot\機械設計\_BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1F3D5D7-5570-40FB-A486-8A8E14811FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:81_{0EAE893C-6ECB-4EB4-B0C2-1C6442D422EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17970" yWindow="13980" windowWidth="14400" windowHeight="10845" xr2:uid="{C1AA427B-3090-4B88-813B-31F0FCCBF5B7}"/>
+    <workbookView xWindow="-17970" yWindow="-2220" windowWidth="14400" windowHeight="10845" xr2:uid="{3A546A70-8406-49F6-8CC8-33629CB94D08}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <customWorkbookViews>
-    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{AE2FF39E-5980-429E-9769-5864CC53C8C4}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="932" windowWidth="960" windowHeight="723" activeSheetId="1"/>
+    <customWorkbookView name="DESKTOP-1 - 個人用ビュー" guid="{49733997-296B-4D47-A299-673F571C89AD}" mergeInterval="0" personalView="1" xWindow="-1198" yWindow="-148" windowWidth="960" windowHeight="723" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -191,12 +191,12 @@
     <t>樹脂ﾜｯｼｬ</t>
   </si>
   <si>
-    <t>R-SA001</t>
-  </si>
-  <si>
     <t>FWSJW-D8-V6-T5.5</t>
   </si>
   <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
     <t>FL678ZZ</t>
   </si>
   <si>
@@ -236,7 +236,7 @@
     <t>RR-HL-RAS001</t>
   </si>
   <si>
-    <t>足単体</t>
+    <t>足単体右半身側</t>
   </si>
   <si>
     <t>材料 &lt;指定なし&gt;</t>
@@ -326,8 +326,13 @@
 </file>
 
 <file path=xl/revisions/revisionHeaders.xml><?xml version="1.0" encoding="utf-8"?>
-<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{6128B02F-973B-4A9C-B8B0-0DC024C05169}">
-  <header guid="{6128B02F-973B-4A9C-B8B0-0DC024C05169}" dateTime="2023-07-12T19:29:29" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+<headers xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac" guid="{FC33C956-4558-483F-992E-4AF3C4C760FC}" diskRevisions="1" revisionId="1" version="2">
+  <header guid="{52555EE7-B9A9-48FB-A2E5-0CDB53F1E2D8}" dateTime="2023-07-13T14:26:18" maxSheetId="2" userName="DESKTOP-1" r:id="rId1">
+    <sheetIdMap count="1">
+      <sheetId val="1"/>
+    </sheetIdMap>
+  </header>
+  <header guid="{FC33C956-4558-483F-992E-4AF3C4C760FC}" dateTime="2023-07-13T14:28:20" maxSheetId="2" userName="DESKTOP-1" r:id="rId2" minRId="1">
     <sheetIdMap count="1">
       <sheetId val="1"/>
     </sheetIdMap>
@@ -337,6 +342,21 @@
 
 <file path=xl/revisions/revisionLog1.xml><?xml version="1.0" encoding="utf-8"?>
 <revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac"/>
+</file>
+
+<file path=xl/revisions/revisionLog2.xml><?xml version="1.0" encoding="utf-8"?>
+<revisions xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <rcc rId="1" sId="1">
+    <oc r="I16" t="inlineStr">
+      <is>
+        <t xml:space="preserve"> </t>
+      </is>
+    </oc>
+    <nc r="I16">
+      <v>3</v>
+    </nc>
+  </rcc>
+</revisions>
 </file>
 
 <file path=xl/revisions/userNames.xml><?xml version="1.0" encoding="utf-8"?>
@@ -639,10 +659,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{550B1809-B5D6-4B8B-A4B6-F39D6ABFF92E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{749069D0-D941-4C77-A7DC-63C2C856A595}">
   <dimension ref="A1:S16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
@@ -1149,16 +1171,14 @@
       <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B12" s="1" t="s">
-        <v>50</v>
-      </c>
+      <c r="B12" s="1"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2" t="s">
         <v>43</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>45</v>
@@ -1166,8 +1186,8 @@
       <c r="H12" s="1">
         <v>1</v>
       </c>
-      <c r="I12" s="1">
-        <v>2</v>
+      <c r="I12" s="1" t="s">
+        <v>51</v>
       </c>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
@@ -1333,7 +1353,7 @@
         <v>3</v>
       </c>
       <c r="I16" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="J16" s="1" t="s">
         <v>67</v>
@@ -1354,7 +1374,7 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{AE2FF39E-5980-429E-9769-5864CC53C8C4}">
+    <customSheetView guid="{49733997-296B-4D47-A299-673F571C89AD}">
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
     </customSheetView>

</xml_diff>